<commit_message>
fixed labels for 15frames, added lr-finder
</commit_message>
<xml_diff>
--- a/data/hh_label.xlsx
+++ b/data/hh_label.xlsx
@@ -250,7 +250,7 @@
     <t xml:space="preserve">4300-20286, 45095-54869, 60184-70685, 128089-134436, 146932-162541, 287701-291595</t>
   </si>
   <si>
-    <t xml:space="preserve">7680-7703, 12203-12223, 63984-64005, 64016-64030, 161323-161342</t>
+    <t xml:space="preserve">7680-7703, 12203-12223, 63984-64005, 64016-64031, 161323-161342</t>
   </si>
   <si>
     <t xml:space="preserve">64170-64229</t>
@@ -433,7 +433,7 @@
     <t xml:space="preserve">0-7001</t>
   </si>
   <si>
-    <t xml:space="preserve">113-137, 160-175, 187-208, 213-231, 247-263, 270-299, 300-327, 382-398, 431-446, 447-468, 538-553, 564-584, 643-794, 858-892, 905-924, 1000-1015, 1069-1093, 1148-1163, 1235-1250, 1261-1278, 1351-1379, 1433-1452, 1529-1550, 1559-1575, 1576-1596, 1600-1624, 1633-1669, 1707-1728, 1746-1783, 2043-2070, 2190-2223, 2256-2338, 2366-2382, 2386-2404, 2412-2451, 2502-2535, 2584-2607, 2615-2648, 2659-2674, 2694-2712, 2739-2774, 2856-2871, 2913-2936, 2986-3019, 3020-3036, 3085-3100, 3110-3125, 3153-3168, 3181-3206, 3272-3294, 3300-3315, 3359-3400, 3401-3416, 3417-3430, 3542-3570, 3589-3604, 3766-3802, 3847-3862, 3896-3916, 3940-3960, 4034-4070, 4283-4298, 4411-4445, 4758-4782, 5327-5354, 5471-5490, 5507-5522, 5575-5591, 5759-5780, 5795-5811, 5853-5868, 5919-5934, 5935-5960, 6019-6050, 6077-6092, 6222-6246, 6438-6453, 6587-6612, 6667-6684, 6768-6787, 6793-6808</t>
+    <t xml:space="preserve">113-137, 160-175, 187-208, 213-231, 247-263, 270-299, 300-327, 382-398, 431-446, 447-468, 538-553, 564-584, 643-794, 858-892, 905-924, 1000-1015, 1069-1093, 1148-1163, 1235-1250, 1261-1278, 1351-1379, 1433-1452, 1529-1550, 1559-1575, 1576-1596, 1600-1624, 1633-1669, 1707-1728, 1746-1783, 2043-2070, 2190-2223, 2256-2338, 2366-2382, 2386-2404, 2412-2451, 2502-2535, 2584-2607, 2615-2648, 2659-2674, 2694-2712, 2739-2774, 2856-2871, 2913-2936, 2986-3019, 3020-3036, 3085-3100, 3110-3125, 3153-3168, 3181-3206, 3272-3294, 3300-3315, 3359-3400, 3401-3430, 3542-3570, 3589-3604, 3766-3802, 3847-3862, 3896-3916, 3940-3960, 4034-4070, 4283-4298, 4411-4445, 4758-4782, 5327-5354, 5471-5490, 5507-5522, 5575-5591, 5759-5780, 5795-5811, 5853-5868, 5919-5934, 5935-5960, 6019-6050, 6077-6092, 6222-6246, 6438-6453, 6587-6612, 6667-6684, 6768-6787, 6793-6808</t>
   </si>
 </sst>
 </file>
@@ -556,23 +556,24 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.9028340080972"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.9959514170041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.7368421052632"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -629,6 +630,13 @@
       <c r="D2" s="1" t="n">
         <v>20181107</v>
       </c>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
       <c r="L2" s="1" t="n">
         <v>30</v>
       </c>
@@ -638,6 +646,7 @@
       <c r="N2" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -667,6 +676,8 @@
       <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
       <c r="L3" s="1" t="n">
         <v>30</v>
       </c>
@@ -676,6 +687,7 @@
       <c r="N3" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -690,6 +702,13 @@
       <c r="D4" s="1" t="n">
         <v>20181116</v>
       </c>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
       <c r="L4" s="1" t="n">
         <v>15</v>
       </c>
@@ -699,6 +718,7 @@
       <c r="N4" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -713,6 +733,13 @@
       <c r="D5" s="1" t="n">
         <v>20181119</v>
       </c>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
       <c r="L5" s="1" t="n">
         <v>15</v>
       </c>
@@ -722,6 +749,7 @@
       <c r="N5" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -751,6 +779,8 @@
       <c r="I6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
       <c r="L6" s="1" t="n">
         <v>15</v>
       </c>
@@ -783,6 +813,11 @@
       <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
       <c r="L7" s="1" t="n">
         <v>15</v>
       </c>
@@ -792,6 +827,7 @@
       <c r="N7" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -812,6 +848,11 @@
       <c r="F8" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
       <c r="L8" s="1" t="n">
         <v>15</v>
       </c>
@@ -821,6 +862,7 @@
       <c r="N8" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -838,12 +880,16 @@
       <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="F9" s="0"/>
       <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
       <c r="L9" s="1" t="n">
         <v>15</v>
       </c>
@@ -879,9 +925,12 @@
       <c r="G10" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="H10" s="0"/>
       <c r="I10" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
       <c r="L10" s="1" t="n">
         <v>15</v>
       </c>
@@ -891,6 +940,7 @@
       <c r="N10" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -908,6 +958,12 @@
       <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
       <c r="L11" s="1" t="n">
         <v>15</v>
       </c>
@@ -917,6 +973,7 @@
       <c r="N11" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -946,6 +1003,8 @@
       <c r="I12" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
       <c r="L12" s="1" t="n">
         <v>15</v>
       </c>
@@ -978,6 +1037,11 @@
       <c r="F13" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
       <c r="L13" s="1" t="n">
         <v>15</v>
       </c>
@@ -987,6 +1051,7 @@
       <c r="N13" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1016,6 +1081,8 @@
       <c r="I14" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
       <c r="L14" s="1" t="n">
         <v>15</v>
       </c>
@@ -1042,9 +1109,15 @@
       <c r="D15" s="1" t="n">
         <v>20181130</v>
       </c>
+      <c r="E15" s="0"/>
       <c r="F15" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
       <c r="L15" s="1" t="n">
         <v>15</v>
       </c>
@@ -1054,6 +1127,7 @@
       <c r="N15" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1068,9 +1142,15 @@
       <c r="D16" s="1" t="n">
         <v>20181129</v>
       </c>
+      <c r="E16" s="0"/>
       <c r="F16" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
       <c r="L16" s="1" t="n">
         <v>15</v>
       </c>
@@ -1080,6 +1160,7 @@
       <c r="N16" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -1094,12 +1175,17 @@
       <c r="D17" s="1" t="n">
         <v>20181130</v>
       </c>
+      <c r="E17" s="0"/>
       <c r="F17" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
       <c r="L17" s="1" t="n">
         <v>15</v>
       </c>
@@ -1109,6 +1195,7 @@
       <c r="N17" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -1135,6 +1222,9 @@
       <c r="H18" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
       <c r="L18" s="1" t="n">
         <v>15</v>
       </c>
@@ -1161,6 +1251,7 @@
       <c r="D19" s="1" t="n">
         <v>20181204</v>
       </c>
+      <c r="E19" s="0"/>
       <c r="F19" s="1" t="s">
         <v>79</v>
       </c>
@@ -1170,6 +1261,9 @@
       <c r="H19" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
       <c r="L19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1179,6 +1273,7 @@
       <c r="N19" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -1193,12 +1288,17 @@
       <c r="D20" s="1" t="n">
         <v>20181206</v>
       </c>
+      <c r="E20" s="0"/>
       <c r="F20" s="1" t="s">
         <v>83</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
       <c r="L20" s="1" t="n">
         <v>15</v>
       </c>
@@ -1231,6 +1331,11 @@
       <c r="F21" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
       <c r="L21" s="1" t="n">
         <v>15</v>
       </c>
@@ -1240,6 +1345,7 @@
       <c r="N21" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1263,6 +1369,10 @@
       <c r="G22" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="H22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
       <c r="L22" s="1" t="n">
         <v>15</v>
       </c>
@@ -1289,12 +1399,17 @@
       <c r="D23" s="1" t="n">
         <v>20181214</v>
       </c>
+      <c r="E23" s="0"/>
       <c r="F23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
       <c r="L23" s="1" t="n">
         <v>15</v>
       </c>
@@ -1304,6 +1419,7 @@
       <c r="N23" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1318,12 +1434,17 @@
       <c r="D24" s="1" t="n">
         <v>20181217</v>
       </c>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
       <c r="G24" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="H24" s="0"/>
       <c r="I24" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
       <c r="L24" s="1" t="n">
         <v>15</v>
       </c>
@@ -1333,6 +1454,7 @@
       <c r="N24" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1353,6 +1475,11 @@
       <c r="F25" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
       <c r="L25" s="1" t="n">
         <v>15</v>
       </c>
@@ -1362,6 +1489,7 @@
       <c r="N25" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -1391,6 +1519,8 @@
       <c r="I26" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
       <c r="L26" s="1" t="n">
         <v>15</v>
       </c>
@@ -1417,9 +1547,14 @@
       <c r="D27" s="1" t="n">
         <v>20181220</v>
       </c>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
       <c r="G27" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="H27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
       <c r="L27" s="1" t="n">
         <v>15</v>
       </c>
@@ -1429,6 +1564,7 @@
       <c r="N27" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -1443,6 +1579,12 @@
       <c r="D28" s="1" t="n">
         <v>20181224</v>
       </c>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
       <c r="L28" s="1" t="n">
         <v>15</v>
       </c>
@@ -1452,6 +1594,7 @@
       <c r="N28" s="1" t="n">
         <v>640</v>
       </c>
+      <c r="O28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -1478,6 +1621,8 @@
       <c r="H29" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
       <c r="L29" s="1" t="n">
         <v>15</v>
       </c>
@@ -1548,6 +1693,8 @@
       <c r="D31" s="1" t="n">
         <v>20181228</v>
       </c>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
       <c r="L31" s="1" t="n">
         <v>15</v>
       </c>
@@ -1571,6 +1718,8 @@
       <c r="D32" s="1" t="n">
         <v>20181231</v>
       </c>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
       <c r="L32" s="1" t="n">
         <v>15</v>
       </c>
@@ -1594,6 +1743,8 @@
       <c r="D33" s="1" t="n">
         <v>20190102</v>
       </c>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
       <c r="L33" s="1" t="n">
         <v>15</v>
       </c>
@@ -1617,6 +1768,8 @@
       <c r="D34" s="1" t="n">
         <v>20190103</v>
       </c>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
       <c r="L34" s="1" t="n">
         <v>15</v>
       </c>
@@ -1640,6 +1793,8 @@
       <c r="D35" s="1" t="n">
         <v>20190110</v>
       </c>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
       <c r="L35" s="1" t="n">
         <v>15</v>
       </c>
@@ -1663,6 +1818,8 @@
       <c r="D36" s="1" t="n">
         <v>20190114</v>
       </c>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
       <c r="L36" s="1" t="n">
         <v>15</v>
       </c>
@@ -1686,6 +1843,8 @@
       <c r="D37" s="1" t="n">
         <v>20190115</v>
       </c>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
       <c r="L37" s="1" t="n">
         <v>15</v>
       </c>
@@ -1709,6 +1868,8 @@
       <c r="D38" s="1" t="n">
         <v>20190117</v>
       </c>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
       <c r="L38" s="1" t="n">
         <v>15</v>
       </c>

</xml_diff>